<commit_message>
Finished all the tests
</commit_message>
<xml_diff>
--- a/map/Clue Map.xlsx
+++ b/map/Clue Map.xlsx
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -293,6 +293,12 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +603,7 @@
   <dimension ref="A1:AP64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +690,9 @@
         <v>17</v>
       </c>
       <c r="Z1" s="3"/>
-      <c r="AA1" s="2"/>
+      <c r="AA1" s="25">
+        <v>0</v>
+      </c>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
@@ -778,7 +786,9 @@
         <v>17</v>
       </c>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="2"/>
+      <c r="AA2" s="25">
+        <v>1</v>
+      </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
@@ -872,7 +882,9 @@
         <v>17</v>
       </c>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="2"/>
+      <c r="AA3" s="25">
+        <v>2</v>
+      </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
@@ -966,7 +978,9 @@
         <v>17</v>
       </c>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="2"/>
+      <c r="AA4" s="25">
+        <v>3</v>
+      </c>
       <c r="AB4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1076,9 @@
         <v>17</v>
       </c>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="2"/>
+      <c r="AA5" s="25">
+        <v>4</v>
+      </c>
       <c r="AB5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1178,9 @@
         <v>17</v>
       </c>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="25">
+        <v>5</v>
+      </c>
       <c r="AB6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1260,7 +1278,9 @@
         <v>17</v>
       </c>
       <c r="Z7" s="3"/>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="25">
+        <v>6</v>
+      </c>
       <c r="AB7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1358,7 +1378,9 @@
         <v>41</v>
       </c>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="2"/>
+      <c r="AA8" s="25">
+        <v>7</v>
+      </c>
       <c r="AB8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1456,7 +1478,9 @@
         <v>18</v>
       </c>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="2"/>
+      <c r="AA9" s="25">
+        <v>8</v>
+      </c>
       <c r="AB9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1556,7 +1580,9 @@
         <v>18</v>
       </c>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="2"/>
+      <c r="AA10" s="25">
+        <v>9</v>
+      </c>
       <c r="AB10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1654,7 +1680,9 @@
         <v>18</v>
       </c>
       <c r="Z11" s="3"/>
-      <c r="AA11" s="2"/>
+      <c r="AA11" s="25">
+        <v>10</v>
+      </c>
       <c r="AB11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +1778,9 @@
         <v>41</v>
       </c>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="2"/>
+      <c r="AA12" s="25">
+        <v>11</v>
+      </c>
       <c r="AB12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1876,9 @@
         <v>41</v>
       </c>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="2"/>
+      <c r="AA13" s="25">
+        <v>12</v>
+      </c>
       <c r="AB13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1942,7 +1974,9 @@
         <v>41</v>
       </c>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="2"/>
+      <c r="AA14" s="25">
+        <v>13</v>
+      </c>
       <c r="AB14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2038,7 +2072,9 @@
         <v>41</v>
       </c>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="2"/>
+      <c r="AA15" s="25">
+        <v>14</v>
+      </c>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
@@ -2132,7 +2168,9 @@
         <v>19</v>
       </c>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="2"/>
+      <c r="AA16" s="25">
+        <v>15</v>
+      </c>
       <c r="AB16" s="2" t="s">
         <v>31</v>
       </c>
@@ -2228,7 +2266,9 @@
         <v>19</v>
       </c>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="2"/>
+      <c r="AA17" s="25">
+        <v>16</v>
+      </c>
       <c r="AB17" s="2" t="s">
         <v>32</v>
       </c>
@@ -2326,7 +2366,9 @@
         <v>19</v>
       </c>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="2"/>
+      <c r="AA18" s="25">
+        <v>17</v>
+      </c>
       <c r="AB18" s="2" t="s">
         <v>33</v>
       </c>
@@ -2422,7 +2464,9 @@
         <v>19</v>
       </c>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="2"/>
+      <c r="AA19" s="25">
+        <v>18</v>
+      </c>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -2516,7 +2560,9 @@
         <v>19</v>
       </c>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="2"/>
+      <c r="AA20" s="25">
+        <v>19</v>
+      </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
@@ -2610,7 +2656,9 @@
         <v>19</v>
       </c>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="2"/>
+      <c r="AA21" s="25">
+        <v>20</v>
+      </c>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
@@ -2672,79 +2720,79 @@
       <c r="AP22" s="2"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="26">
         <v>0</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="26">
         <v>1</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="26">
         <v>2</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="26">
         <v>3</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="26">
         <v>4</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="26">
         <v>5</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="26">
         <v>6</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="26">
         <v>7</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="26">
         <v>8</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="26">
         <v>9</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="26">
         <v>10</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="26">
         <v>11</v>
       </c>
-      <c r="M23" s="2">
-        <v>12</v>
-      </c>
-      <c r="N23" s="2">
+      <c r="M23" s="26">
+        <v>12</v>
+      </c>
+      <c r="N23" s="26">
         <v>13</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="26">
         <v>14</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23" s="26">
         <v>15</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q23" s="26">
         <v>16</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R23" s="26">
         <v>17</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="26">
         <v>18</v>
       </c>
-      <c r="T23" s="2">
-        <v>19</v>
-      </c>
-      <c r="U23" s="2">
+      <c r="T23" s="26">
+        <v>19</v>
+      </c>
+      <c r="U23" s="26">
         <v>20</v>
       </c>
-      <c r="V23" s="2">
+      <c r="V23" s="26">
         <v>21</v>
       </c>
-      <c r="W23" s="2">
+      <c r="W23" s="26">
         <v>22</v>
       </c>
-      <c r="X23" s="2">
+      <c r="X23" s="26">
         <v>23</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Y23" s="26">
         <v>24</v>
       </c>
       <c r="Z23" s="2"/>

</xml_diff>

<commit_message>
Got rid of panelSize and roomPrintNames
</commit_message>
<xml_diff>
--- a/map/Clue Map.xlsx
+++ b/map/Clue Map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="53">
   <si>
     <t>Key</t>
   </si>
@@ -145,6 +145,36 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>sN</t>
+  </si>
+  <si>
+    <t>mN</t>
+  </si>
+  <si>
+    <t>iN</t>
+  </si>
+  <si>
+    <t>aN</t>
+  </si>
+  <si>
+    <t>zN</t>
+  </si>
+  <si>
+    <t>yN</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>dN</t>
+  </si>
+  <si>
+    <t>rN</t>
+  </si>
+  <si>
+    <t>pN</t>
   </si>
 </sst>
 </file>
@@ -603,7 +633,7 @@
   <dimension ref="A1:AP64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>14</v>
@@ -831,7 +861,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>15</v>
@@ -852,7 +882,7 @@
         <v>16</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="Q3" s="16" t="s">
         <v>16</v>
@@ -969,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="W4" s="17" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="X4" s="17" t="s">
         <v>17</v>
@@ -1565,7 +1595,7 @@
         <v>18</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="V10" s="20" t="s">
         <v>18</v>
@@ -1641,7 +1671,7 @@
         <v>42</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N11" s="19" t="s">
         <v>42</v>
@@ -1706,7 +1736,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>11</v>
@@ -2398,7 +2428,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>12</v>
@@ -2425,7 +2455,7 @@
         <v>13</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="N19" s="21" t="s">
         <v>13</v>
@@ -2539,7 +2569,7 @@
         <v>19</v>
       </c>
       <c r="S20" s="23" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="T20" s="23" t="s">
         <v>19</v>

</xml_diff>